<commit_message>
Fix cell size with set_row_pixels & set_column_pixels. Add  auto libreoffice start (works only o my machine, no crossplatofrm)
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -444,10 +444,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="120" width="1.7109375" customWidth="1"/>
+    <col min="1" max="120" width="2.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:119" ht="4" customHeight="1">
+    <row r="1" spans="1:119" ht="12" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -568,7 +568,7 @@
       <c r="DN1" s="1"/>
       <c r="DO1" s="1"/>
     </row>
-    <row r="2" spans="1:119" ht="4" customHeight="1">
+    <row r="2" spans="1:119" ht="12" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -689,7 +689,7 @@
       <c r="DN2" s="1"/>
       <c r="DO2" s="1"/>
     </row>
-    <row r="3" spans="1:119" ht="4" customHeight="1">
+    <row r="3" spans="1:119" ht="12" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -810,7 +810,7 @@
       <c r="DN3" s="1"/>
       <c r="DO3" s="1"/>
     </row>
-    <row r="4" spans="1:119" ht="4" customHeight="1">
+    <row r="4" spans="1:119" ht="12" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -931,7 +931,7 @@
       <c r="DN4" s="1"/>
       <c r="DO4" s="1"/>
     </row>
-    <row r="5" spans="1:119" ht="4" customHeight="1">
+    <row r="5" spans="1:119" ht="12" customHeight="1">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1052,7 +1052,7 @@
       <c r="DN5" s="1"/>
       <c r="DO5" s="1"/>
     </row>
-    <row r="6" spans="1:119" ht="4" customHeight="1">
+    <row r="6" spans="1:119" ht="12" customHeight="1">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1173,7 +1173,7 @@
       <c r="DN6" s="1"/>
       <c r="DO6" s="1"/>
     </row>
-    <row r="7" spans="1:119" ht="4" customHeight="1">
+    <row r="7" spans="1:119" ht="12" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1294,7 +1294,7 @@
       <c r="DN7" s="1"/>
       <c r="DO7" s="1"/>
     </row>
-    <row r="8" spans="1:119" ht="4" customHeight="1">
+    <row r="8" spans="1:119" ht="12" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1415,7 +1415,7 @@
       <c r="DN8" s="1"/>
       <c r="DO8" s="1"/>
     </row>
-    <row r="9" spans="1:119" ht="4" customHeight="1">
+    <row r="9" spans="1:119" ht="12" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1536,7 +1536,7 @@
       <c r="DN9" s="1"/>
       <c r="DO9" s="1"/>
     </row>
-    <row r="10" spans="1:119" ht="4" customHeight="1">
+    <row r="10" spans="1:119" ht="12" customHeight="1">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1657,7 +1657,7 @@
       <c r="DN10" s="1"/>
       <c r="DO10" s="1"/>
     </row>
-    <row r="11" spans="1:119" ht="4" customHeight="1">
+    <row r="11" spans="1:119" ht="12" customHeight="1">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1778,7 +1778,7 @@
       <c r="DN11" s="1"/>
       <c r="DO11" s="1"/>
     </row>
-    <row r="12" spans="1:119" ht="4" customHeight="1">
+    <row r="12" spans="1:119" ht="12" customHeight="1">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1899,7 +1899,7 @@
       <c r="DN12" s="1"/>
       <c r="DO12" s="1"/>
     </row>
-    <row r="13" spans="1:119" ht="4" customHeight="1">
+    <row r="13" spans="1:119" ht="12" customHeight="1">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -2020,7 +2020,7 @@
       <c r="DN13" s="1"/>
       <c r="DO13" s="1"/>
     </row>
-    <row r="14" spans="1:119" ht="4" customHeight="1">
+    <row r="14" spans="1:119" ht="12" customHeight="1">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -2141,7 +2141,7 @@
       <c r="DN14" s="1"/>
       <c r="DO14" s="1"/>
     </row>
-    <row r="15" spans="1:119" ht="4" customHeight="1">
+    <row r="15" spans="1:119" ht="12" customHeight="1">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2262,7 +2262,7 @@
       <c r="DN15" s="1"/>
       <c r="DO15" s="1"/>
     </row>
-    <row r="16" spans="1:119" ht="4" customHeight="1">
+    <row r="16" spans="1:119" ht="12" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -2383,7 +2383,7 @@
       <c r="DN16" s="1"/>
       <c r="DO16" s="1"/>
     </row>
-    <row r="17" spans="1:119" ht="4" customHeight="1">
+    <row r="17" spans="1:119" ht="12" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2504,7 +2504,7 @@
       <c r="DN17" s="1"/>
       <c r="DO17" s="1"/>
     </row>
-    <row r="18" spans="1:119" ht="4" customHeight="1">
+    <row r="18" spans="1:119" ht="12" customHeight="1">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2625,7 +2625,7 @@
       <c r="DN18" s="1"/>
       <c r="DO18" s="1"/>
     </row>
-    <row r="19" spans="1:119" ht="4" customHeight="1">
+    <row r="19" spans="1:119" ht="12" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -2746,7 +2746,7 @@
       <c r="DN19" s="1"/>
       <c r="DO19" s="1"/>
     </row>
-    <row r="20" spans="1:119" ht="4" customHeight="1">
+    <row r="20" spans="1:119" ht="12" customHeight="1">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -2867,7 +2867,7 @@
       <c r="DN20" s="1"/>
       <c r="DO20" s="1"/>
     </row>
-    <row r="21" spans="1:119" ht="4" customHeight="1">
+    <row r="21" spans="1:119" ht="12" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -2988,7 +2988,7 @@
       <c r="DN21" s="1"/>
       <c r="DO21" s="1"/>
     </row>
-    <row r="22" spans="1:119" ht="4" customHeight="1">
+    <row r="22" spans="1:119" ht="12" customHeight="1">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -3109,7 +3109,7 @@
       <c r="DN22" s="1"/>
       <c r="DO22" s="1"/>
     </row>
-    <row r="23" spans="1:119" ht="4" customHeight="1">
+    <row r="23" spans="1:119" ht="12" customHeight="1">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -3230,7 +3230,7 @@
       <c r="DN23" s="1"/>
       <c r="DO23" s="1"/>
     </row>
-    <row r="24" spans="1:119" ht="4" customHeight="1">
+    <row r="24" spans="1:119" ht="12" customHeight="1">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -3351,7 +3351,7 @@
       <c r="DN24" s="1"/>
       <c r="DO24" s="1"/>
     </row>
-    <row r="25" spans="1:119" ht="4" customHeight="1">
+    <row r="25" spans="1:119" ht="12" customHeight="1">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -3472,7 +3472,7 @@
       <c r="DN25" s="1"/>
       <c r="DO25" s="1"/>
     </row>
-    <row r="26" spans="1:119" ht="4" customHeight="1">
+    <row r="26" spans="1:119" ht="12" customHeight="1">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -3593,7 +3593,7 @@
       <c r="DN26" s="1"/>
       <c r="DO26" s="1"/>
     </row>
-    <row r="27" spans="1:119" ht="4" customHeight="1">
+    <row r="27" spans="1:119" ht="12" customHeight="1">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -3714,7 +3714,7 @@
       <c r="DN27" s="1"/>
       <c r="DO27" s="1"/>
     </row>
-    <row r="28" spans="1:119" ht="4" customHeight="1">
+    <row r="28" spans="1:119" ht="12" customHeight="1">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
@@ -3835,7 +3835,7 @@
       <c r="DN28" s="1"/>
       <c r="DO28" s="1"/>
     </row>
-    <row r="29" spans="1:119" ht="4" customHeight="1">
+    <row r="29" spans="1:119" ht="12" customHeight="1">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
@@ -3956,7 +3956,7 @@
       <c r="DN29" s="1"/>
       <c r="DO29" s="1"/>
     </row>
-    <row r="30" spans="1:119" ht="4" customHeight="1">
+    <row r="30" spans="1:119" ht="12" customHeight="1">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -4077,7 +4077,7 @@
       <c r="DN30" s="1"/>
       <c r="DO30" s="1"/>
     </row>
-    <row r="31" spans="1:119" ht="4" customHeight="1">
+    <row r="31" spans="1:119" ht="12" customHeight="1">
       <c r="A31" s="9"/>
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
@@ -4198,7 +4198,7 @@
       <c r="DN31" s="1"/>
       <c r="DO31" s="1"/>
     </row>
-    <row r="32" spans="1:119" ht="4" customHeight="1">
+    <row r="32" spans="1:119" ht="12" customHeight="1">
       <c r="A32" s="9"/>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
@@ -4319,7 +4319,7 @@
       <c r="DN32" s="1"/>
       <c r="DO32" s="1"/>
     </row>
-    <row r="33" spans="1:119" ht="4" customHeight="1">
+    <row r="33" spans="1:119" ht="12" customHeight="1">
       <c r="A33" s="9"/>
       <c r="B33" s="9"/>
       <c r="C33" s="9"/>
@@ -4440,7 +4440,7 @@
       <c r="DN33" s="1"/>
       <c r="DO33" s="1"/>
     </row>
-    <row r="34" spans="1:119" ht="4" customHeight="1">
+    <row r="34" spans="1:119" ht="12" customHeight="1">
       <c r="A34" s="11"/>
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
@@ -4561,7 +4561,7 @@
       <c r="DN34" s="1"/>
       <c r="DO34" s="1"/>
     </row>
-    <row r="35" spans="1:119" ht="4" customHeight="1">
+    <row r="35" spans="1:119" ht="12" customHeight="1">
       <c r="A35" s="11"/>
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
@@ -4682,7 +4682,7 @@
       <c r="DN35" s="1"/>
       <c r="DO35" s="1"/>
     </row>
-    <row r="36" spans="1:119" ht="4" customHeight="1">
+    <row r="36" spans="1:119" ht="12" customHeight="1">
       <c r="A36" s="11"/>
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
@@ -4803,7 +4803,7 @@
       <c r="DN36" s="1"/>
       <c r="DO36" s="1"/>
     </row>
-    <row r="37" spans="1:119" ht="4" customHeight="1">
+    <row r="37" spans="1:119" ht="12" customHeight="1">
       <c r="A37" s="12"/>
       <c r="B37" s="12"/>
       <c r="C37" s="12"/>
@@ -4924,7 +4924,7 @@
       <c r="DN37" s="1"/>
       <c r="DO37" s="1"/>
     </row>
-    <row r="38" spans="1:119" ht="4" customHeight="1">
+    <row r="38" spans="1:119" ht="12" customHeight="1">
       <c r="A38" s="12"/>
       <c r="B38" s="12"/>
       <c r="C38" s="12"/>
@@ -5045,7 +5045,7 @@
       <c r="DN38" s="1"/>
       <c r="DO38" s="1"/>
     </row>
-    <row r="39" spans="1:119" ht="4" customHeight="1">
+    <row r="39" spans="1:119" ht="12" customHeight="1">
       <c r="A39" s="12"/>
       <c r="B39" s="12"/>
       <c r="C39" s="12"/>
@@ -5166,7 +5166,7 @@
       <c r="DN39" s="1"/>
       <c r="DO39" s="1"/>
     </row>
-    <row r="40" spans="1:119" ht="4" customHeight="1">
+    <row r="40" spans="1:119" ht="12" customHeight="1">
       <c r="A40" s="14"/>
       <c r="B40" s="14"/>
       <c r="C40" s="14"/>
@@ -5287,7 +5287,7 @@
       <c r="DN40" s="1"/>
       <c r="DO40" s="1"/>
     </row>
-    <row r="41" spans="1:119" ht="4" customHeight="1">
+    <row r="41" spans="1:119" ht="12" customHeight="1">
       <c r="A41" s="14"/>
       <c r="B41" s="14"/>
       <c r="C41" s="14"/>
@@ -5408,7 +5408,7 @@
       <c r="DN41" s="1"/>
       <c r="DO41" s="1"/>
     </row>
-    <row r="42" spans="1:119" ht="4" customHeight="1">
+    <row r="42" spans="1:119" ht="12" customHeight="1">
       <c r="A42" s="14"/>
       <c r="B42" s="14"/>
       <c r="C42" s="14"/>
@@ -5529,7 +5529,7 @@
       <c r="DN42" s="1"/>
       <c r="DO42" s="1"/>
     </row>
-    <row r="43" spans="1:119" ht="4" customHeight="1">
+    <row r="43" spans="1:119" ht="12" customHeight="1">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -5650,7 +5650,7 @@
       <c r="DN43" s="1"/>
       <c r="DO43" s="1"/>
     </row>
-    <row r="44" spans="1:119" ht="4" customHeight="1">
+    <row r="44" spans="1:119" ht="12" customHeight="1">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -5771,7 +5771,7 @@
       <c r="DN44" s="1"/>
       <c r="DO44" s="1"/>
     </row>
-    <row r="45" spans="1:119" ht="4" customHeight="1">
+    <row r="45" spans="1:119" ht="12" customHeight="1">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -5892,7 +5892,7 @@
       <c r="DN45" s="1"/>
       <c r="DO45" s="1"/>
     </row>
-    <row r="46" spans="1:119" ht="4" customHeight="1">
+    <row r="46" spans="1:119" ht="12" customHeight="1">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -6013,7 +6013,7 @@
       <c r="DN46" s="1"/>
       <c r="DO46" s="1"/>
     </row>
-    <row r="47" spans="1:119" ht="4" customHeight="1">
+    <row r="47" spans="1:119" ht="12" customHeight="1">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -6134,7 +6134,7 @@
       <c r="DN47" s="1"/>
       <c r="DO47" s="1"/>
     </row>
-    <row r="48" spans="1:119" ht="4" customHeight="1">
+    <row r="48" spans="1:119" ht="12" customHeight="1">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -6255,7 +6255,7 @@
       <c r="DN48" s="1"/>
       <c r="DO48" s="1"/>
     </row>
-    <row r="49" spans="1:119" ht="4" customHeight="1">
+    <row r="49" spans="1:119" ht="12" customHeight="1">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -6376,7 +6376,7 @@
       <c r="DN49" s="1"/>
       <c r="DO49" s="1"/>
     </row>
-    <row r="50" spans="1:119" ht="4" customHeight="1">
+    <row r="50" spans="1:119" ht="12" customHeight="1">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -6497,7 +6497,7 @@
       <c r="DN50" s="1"/>
       <c r="DO50" s="1"/>
     </row>
-    <row r="51" spans="1:119" ht="4" customHeight="1">
+    <row r="51" spans="1:119" ht="12" customHeight="1">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -6618,7 +6618,7 @@
       <c r="DN51" s="1"/>
       <c r="DO51" s="1"/>
     </row>
-    <row r="52" spans="1:119" ht="4" customHeight="1">
+    <row r="52" spans="1:119" ht="12" customHeight="1">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -6739,7 +6739,7 @@
       <c r="DN52" s="1"/>
       <c r="DO52" s="1"/>
     </row>
-    <row r="53" spans="1:119" ht="4" customHeight="1">
+    <row r="53" spans="1:119" ht="12" customHeight="1">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -6860,7 +6860,7 @@
       <c r="DN53" s="1"/>
       <c r="DO53" s="1"/>
     </row>
-    <row r="54" spans="1:119" ht="4" customHeight="1">
+    <row r="54" spans="1:119" ht="12" customHeight="1">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -6981,7 +6981,7 @@
       <c r="DN54" s="1"/>
       <c r="DO54" s="1"/>
     </row>
-    <row r="55" spans="1:119" ht="4" customHeight="1">
+    <row r="55" spans="1:119" ht="12" customHeight="1">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -7102,7 +7102,7 @@
       <c r="DN55" s="1"/>
       <c r="DO55" s="1"/>
     </row>
-    <row r="56" spans="1:119" ht="4" customHeight="1">
+    <row r="56" spans="1:119" ht="12" customHeight="1">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -7223,7 +7223,7 @@
       <c r="DN56" s="1"/>
       <c r="DO56" s="1"/>
     </row>
-    <row r="57" spans="1:119" ht="4" customHeight="1">
+    <row r="57" spans="1:119" ht="12" customHeight="1">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -7344,7 +7344,7 @@
       <c r="DN57" s="1"/>
       <c r="DO57" s="1"/>
     </row>
-    <row r="58" spans="1:119" ht="4" customHeight="1">
+    <row r="58" spans="1:119" ht="12" customHeight="1">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -7465,7 +7465,7 @@
       <c r="DN58" s="1"/>
       <c r="DO58" s="1"/>
     </row>
-    <row r="59" spans="1:119" ht="4" customHeight="1">
+    <row r="59" spans="1:119" ht="12" customHeight="1">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -7586,7 +7586,7 @@
       <c r="DN59" s="1"/>
       <c r="DO59" s="1"/>
     </row>
-    <row r="60" spans="1:119" ht="4" customHeight="1">
+    <row r="60" spans="1:119" ht="12" customHeight="1">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -7707,7 +7707,7 @@
       <c r="DN60" s="1"/>
       <c r="DO60" s="1"/>
     </row>
-    <row r="61" spans="1:119" ht="4" customHeight="1">
+    <row r="61" spans="1:119" ht="12" customHeight="1">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -7828,7 +7828,7 @@
       <c r="DN61" s="1"/>
       <c r="DO61" s="1"/>
     </row>
-    <row r="62" spans="1:119" ht="4" customHeight="1">
+    <row r="62" spans="1:119" ht="12" customHeight="1">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -7949,7 +7949,7 @@
       <c r="DN62" s="1"/>
       <c r="DO62" s="1"/>
     </row>
-    <row r="63" spans="1:119" ht="4" customHeight="1">
+    <row r="63" spans="1:119" ht="12" customHeight="1">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -8070,7 +8070,7 @@
       <c r="DN63" s="1"/>
       <c r="DO63" s="1"/>
     </row>
-    <row r="64" spans="1:119" ht="4" customHeight="1">
+    <row r="64" spans="1:119" ht="12" customHeight="1">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -8191,7 +8191,7 @@
       <c r="DN64" s="1"/>
       <c r="DO64" s="1"/>
     </row>
-    <row r="65" spans="1:119" ht="4" customHeight="1">
+    <row r="65" spans="1:119" ht="12" customHeight="1">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -8312,7 +8312,7 @@
       <c r="DN65" s="1"/>
       <c r="DO65" s="1"/>
     </row>
-    <row r="66" spans="1:119" ht="4" customHeight="1">
+    <row r="66" spans="1:119" ht="12" customHeight="1">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -8433,7 +8433,7 @@
       <c r="DN66" s="1"/>
       <c r="DO66" s="1"/>
     </row>
-    <row r="67" spans="1:119" ht="4" customHeight="1">
+    <row r="67" spans="1:119" ht="12" customHeight="1">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -8554,7 +8554,7 @@
       <c r="DN67" s="1"/>
       <c r="DO67" s="1"/>
     </row>
-    <row r="68" spans="1:119" ht="4" customHeight="1">
+    <row r="68" spans="1:119" ht="12" customHeight="1">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -8675,7 +8675,7 @@
       <c r="DN68" s="1"/>
       <c r="DO68" s="1"/>
     </row>
-    <row r="69" spans="1:119" ht="4" customHeight="1">
+    <row r="69" spans="1:119" ht="12" customHeight="1">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -8796,7 +8796,7 @@
       <c r="DN69" s="1"/>
       <c r="DO69" s="1"/>
     </row>
-    <row r="70" spans="1:119" ht="4" customHeight="1">
+    <row r="70" spans="1:119" ht="12" customHeight="1">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>

</xml_diff>